<commit_message>
Update Usuário Logado - thiago-pinheiro.xlsx
</commit_message>
<xml_diff>
--- a/softwares_instalados/Usuário Logado - thiago-pinheiro.xlsx
+++ b/softwares_instalados/Usuário Logado - thiago-pinheiro.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="158">
   <si>
     <t>DisplayName</t>
   </si>
@@ -494,16 +494,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -519,7 +511,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -527,30 +519,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,6 +532,17 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TabelaSoftware" displayName="TabelaSoftware" ref="A1:B99" totalsRowShown="0">
+  <autoFilter ref="A1:B99"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="DisplayName"/>
+    <tableColumn id="2" name="DisplayVersion"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -847,18 +832,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="80.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1645,5 +1634,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>